<commit_message>
Update trees and efficiency curve plot
</commit_message>
<xml_diff>
--- a/models/markov.xlsx
+++ b/models/markov.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\david\anus\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BEC0FBE-AF16-497C-9B37-3E3191ED23BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B5AC79-B917-49B3-9686-73AF5CDEAA90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1050" windowWidth="21840" windowHeight="13740" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -131,15 +131,9 @@
     <t>p_death_other</t>
   </si>
   <si>
-    <t>p_no_hsil___semestral_followup</t>
-  </si>
-  <si>
     <t>p_cancer___semestral_followup</t>
   </si>
   <si>
-    <t>p_survive</t>
-  </si>
-  <si>
     <t>p_death_cancer</t>
   </si>
   <si>
@@ -173,9 +167,6 @@
     <t>p_undetected_cancer</t>
   </si>
   <si>
-    <t>p_no_hsil___semestral_followup_undetected</t>
-  </si>
-  <si>
     <t>p_cancer___semestral_followup_undetected</t>
   </si>
   <si>
@@ -189,6 +180,15 @@
   </si>
   <si>
     <t>p_detected_cancer___undetected</t>
+  </si>
+  <si>
+    <t>c_surgery</t>
+  </si>
+  <si>
+    <t>p_hsil___semestral_followup</t>
+  </si>
+  <si>
+    <t>p_hsil___semestral_followup_undetected</t>
   </si>
 </sst>
 </file>
@@ -549,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -619,10 +619,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -633,10 +633,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -652,8 +652,8 @@
       <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C7">
-        <v>0</v>
+      <c r="C7" t="s">
+        <v>47</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
@@ -661,16 +661,16 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
         <v>35</v>
-      </c>
-      <c r="B8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -730,7 +730,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -761,16 +761,16 @@
         <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G1" t="s">
         <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I1" t="s">
         <v>16</v>
@@ -832,12 +832,12 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -856,7 +856,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -897,16 +897,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G9" sqref="G9"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.453125" customWidth="1"/>
     <col min="2" max="2" width="12.90625" customWidth="1"/>
-    <col min="3" max="3" width="18.81640625" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
     <col min="4" max="4" width="19.453125" customWidth="1"/>
     <col min="5" max="5" width="34.453125" customWidth="1"/>
     <col min="6" max="6" width="22.08984375" customWidth="1"/>
@@ -932,16 +932,16 @@
         <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G1" t="s">
         <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I1" t="s">
         <v>16</v>
@@ -967,16 +967,16 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1060,7 +1060,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1095,7 +1095,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1165,7 +1165,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1177,13 +1177,13 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H8" t="s">
         <v>27</v>
@@ -1317,17 +1317,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0EB2218-1218-4D74-BE4B-A50C70982977}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.453125" customWidth="1"/>
-    <col min="2" max="2" width="12.90625" customWidth="1"/>
-    <col min="3" max="3" width="18.81640625" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" customWidth="1"/>
+    <col min="1" max="1" width="45.36328125" customWidth="1"/>
+    <col min="2" max="2" width="26.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.26953125" customWidth="1"/>
     <col min="5" max="5" width="34.453125" customWidth="1"/>
     <col min="6" max="6" width="22.08984375" customWidth="1"/>
     <col min="7" max="7" width="37.1796875" customWidth="1"/>
@@ -1352,16 +1352,16 @@
         <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G1" t="s">
         <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I1" t="s">
         <v>16</v>
@@ -1416,19 +1416,19 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
         <v>30</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3" t="s">
-        <v>31</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -1448,22 +1448,22 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
         <v>30</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>31</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1480,7 +1480,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1492,13 +1492,13 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" t="s">
         <v>27</v>
       </c>
-      <c r="F5" t="s">
-        <v>44</v>
-      </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -1507,7 +1507,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K5" t="s">
         <v>29</v>
@@ -1515,7 +1515,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1527,22 +1527,22 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" t="s">
         <v>27</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" t="s">
-        <v>44</v>
-      </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K6" t="s">
         <v>29</v>
@@ -1567,17 +1567,17 @@
       <c r="F7">
         <v>0</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
         <v>27</v>
       </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7" t="s">
-        <v>32</v>
-      </c>
       <c r="J7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K7" t="s">
         <v>29</v>
@@ -1585,7 +1585,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1612,7 +1612,7 @@
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K8" t="s">
         <v>29</v>
@@ -1638,7 +1638,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H9">
         <v>0</v>

</xml_diff>

<commit_message>
Fix and refactor for first presented results
</commit_message>
<xml_diff>
--- a/models/markov.xlsx
+++ b/models/markov.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\david\anus\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F57C934-B7B9-4C89-B076-8CA365B45A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0051CCF-BD26-4130-BA49-6F9AA3AACB01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="46680" yWindow="2790" windowWidth="19440" windowHeight="15600" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>hiv_positive</t>
   </si>
   <si>
-    <t>MSM, HIV+</t>
-  </si>
-  <si>
     <t>u_hiv_p</t>
   </si>
   <si>
@@ -254,12 +251,6 @@
     <t>undetected_hsil_annual_followup2</t>
   </si>
   <si>
-    <t>MSM, HIV+ (waiting for next annual followup, 12 months remaining)</t>
-  </si>
-  <si>
-    <t>MSM, HIV+ (waiting for next annual followup, 6 months remaining)</t>
-  </si>
-  <si>
     <t>Undetected HSIL (waiting for next annual followup, 12 months remaining)</t>
   </si>
   <si>
@@ -279,13 +270,55 @@
   </si>
   <si>
     <t>p_hsil_regression___semestral_followup_hsil_irc</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MSM, HIV+ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(no HSIL)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MSM, HIV+ (waiting for next annual followup, 6 months remaining) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(no HSIL)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MSM, HIV+ (waiting for next annual followup, 12 months remaining) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(no HSIL)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -305,6 +338,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -648,13 +687,13 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.5703125" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
   </cols>
@@ -678,245 +717,245 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
         <v>7</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
         <v>8</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
         <v>10</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
         <v>11</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" t="s">
         <v>57</v>
       </c>
-      <c r="B18" t="s">
-        <v>58</v>
-      </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
         <v>13</v>
-      </c>
-      <c r="B19" t="s">
-        <v>14</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -927,10 +966,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
         <v>15</v>
-      </c>
-      <c r="B20" t="s">
-        <v>16</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -941,7 +980,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -983,58 +1022,58 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" t="s">
         <v>69</v>
       </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G1" t="s">
-        <v>70</v>
-      </c>
       <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" t="s">
-        <v>32</v>
-      </c>
       <c r="J1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" t="s">
         <v>29</v>
       </c>
-      <c r="K1" t="s">
-        <v>30</v>
-      </c>
       <c r="L1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" t="s">
         <v>43</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>44</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>45</v>
       </c>
-      <c r="O1" t="s">
-        <v>46</v>
-      </c>
       <c r="P1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="R1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="S1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -1042,133 +1081,133 @@
         <v>4</v>
       </c>
       <c r="T2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="T5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="T9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="T10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="T11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="S16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="T16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1186,8 +1225,8 @@
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M17" sqref="M17"/>
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1223,58 +1262,58 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" t="s">
         <v>69</v>
       </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G1" t="s">
-        <v>70</v>
-      </c>
       <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" t="s">
-        <v>32</v>
-      </c>
       <c r="J1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" t="s">
         <v>29</v>
       </c>
-      <c r="K1" t="s">
-        <v>30</v>
-      </c>
       <c r="L1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" t="s">
         <v>43</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>44</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>45</v>
       </c>
-      <c r="O1" t="s">
-        <v>46</v>
-      </c>
       <c r="P1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="R1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="S1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -1285,7 +1324,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1300,7 +1339,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1312,7 +1351,7 @@
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -1330,7 +1369,7 @@
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S2">
         <v>0</v>
@@ -1341,7 +1380,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1403,7 +1442,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1465,7 +1504,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1480,7 +1519,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -1492,7 +1531,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -1504,19 +1543,19 @@
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q5">
         <v>0</v>
       </c>
       <c r="R5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S5">
         <v>0</v>
@@ -1527,7 +1566,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1589,7 +1628,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1651,7 +1690,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1672,10 +1711,10 @@
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -1684,7 +1723,7 @@
         <v>0</v>
       </c>
       <c r="L8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -1702,7 +1741,7 @@
         <v>0</v>
       </c>
       <c r="R8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S8">
         <v>0</v>
@@ -1713,10 +1752,10 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1734,7 +1773,7 @@
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -1746,7 +1785,7 @@
         <v>0</v>
       </c>
       <c r="L9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -1764,7 +1803,7 @@
         <v>0</v>
       </c>
       <c r="R9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S9">
         <v>0</v>
@@ -1775,7 +1814,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1802,10 +1841,10 @@
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -1814,19 +1853,19 @@
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q10">
         <v>0</v>
       </c>
       <c r="R10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S10">
         <v>0</v>
@@ -1837,7 +1876,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1849,7 +1888,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1864,7 +1903,7 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -1876,19 +1915,19 @@
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O11">
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q11">
         <v>0</v>
       </c>
       <c r="R11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S11">
         <v>0</v>
@@ -1899,7 +1938,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1932,10 +1971,10 @@
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N12">
         <v>0</v>
@@ -1950,7 +1989,7 @@
         <v>0</v>
       </c>
       <c r="R12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S12">
         <v>0</v>
@@ -1961,10 +2000,10 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1994,7 +2033,7 @@
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -2012,7 +2051,7 @@
         <v>0</v>
       </c>
       <c r="R13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S13">
         <v>0</v>
@@ -2023,7 +2062,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -2062,19 +2101,19 @@
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q14">
         <v>0</v>
       </c>
       <c r="R14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="S14">
         <v>0</v>
@@ -2085,7 +2124,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -2097,7 +2136,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -2124,19 +2163,19 @@
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q15">
         <v>0</v>
       </c>
       <c r="R15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="S15">
         <v>0</v>
@@ -2147,7 +2186,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -2209,7 +2248,7 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -2271,7 +2310,7 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -2333,7 +2372,7 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -2395,7 +2434,7 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -2470,8 +2509,8 @@
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C5" sqref="C5"/>
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2501,58 +2540,58 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" t="s">
         <v>69</v>
       </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G1" t="s">
-        <v>70</v>
-      </c>
       <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" t="s">
-        <v>32</v>
-      </c>
       <c r="J1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" t="s">
         <v>29</v>
       </c>
-      <c r="K1" t="s">
-        <v>30</v>
-      </c>
       <c r="L1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" t="s">
         <v>43</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>44</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>45</v>
       </c>
-      <c r="O1" t="s">
-        <v>46</v>
-      </c>
       <c r="P1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="R1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="S1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -2560,66 +2599,66 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2" t="s">
         <v>19</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2628,125 +2667,125 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3" t="s">
         <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4" t="s">
         <v>19</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -2755,60 +2794,60 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5" t="s">
         <v>19</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -2823,54 +2862,54 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6" t="s">
         <v>19</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -2879,57 +2918,57 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7" t="s">
         <v>19</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2950,48 +2989,48 @@
         <v>0</v>
       </c>
       <c r="H8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8" t="s">
+        <v>37</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8" t="s">
         <v>19</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8" t="s">
-        <v>38</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -3015,45 +3054,45 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9" t="s">
         <v>19</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9" t="s">
-        <v>38</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-      <c r="T9" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -3074,48 +3113,48 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10" t="s">
         <v>19</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-      <c r="T10" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -3139,45 +3178,45 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J11">
         <v>0</v>
       </c>
       <c r="K11" t="s">
+        <v>18</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11" t="s">
         <v>19</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -3210,36 +3249,36 @@
         <v>0</v>
       </c>
       <c r="L12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12" t="s">
+        <v>52</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12" t="s">
         <v>19</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12" t="s">
-        <v>53</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-      <c r="R12">
-        <v>0</v>
-      </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
-      <c r="T12" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -3275,33 +3314,33 @@
         <v>0</v>
       </c>
       <c r="M13" t="s">
+        <v>18</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13" t="s">
+        <v>52</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13" t="s">
         <v>19</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13" t="s">
-        <v>53</v>
-      </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-      <c r="R13">
-        <v>0</v>
-      </c>
-      <c r="S13">
-        <v>0</v>
-      </c>
-      <c r="T13" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -3334,36 +3373,36 @@
         <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
       <c r="N14" t="s">
+        <v>18</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14" t="s">
         <v>19</v>
-      </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
-      <c r="Q14">
-        <v>0</v>
-      </c>
-      <c r="R14">
-        <v>0</v>
-      </c>
-      <c r="S14">
-        <v>0</v>
-      </c>
-      <c r="T14" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -3399,33 +3438,33 @@
         <v>0</v>
       </c>
       <c r="M15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="N15">
         <v>0</v>
       </c>
       <c r="O15" t="s">
+        <v>18</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15" t="s">
         <v>19</v>
-      </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
-      <c r="R15">
-        <v>0</v>
-      </c>
-      <c r="S15">
-        <v>0</v>
-      </c>
-      <c r="T15" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -3470,24 +3509,24 @@
         <v>0</v>
       </c>
       <c r="P16" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>41</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16" t="s">
+        <v>20</v>
+      </c>
+      <c r="T16" t="s">
         <v>19</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>42</v>
-      </c>
-      <c r="R16">
-        <v>0</v>
-      </c>
-      <c r="S16" t="s">
-        <v>21</v>
-      </c>
-      <c r="T16" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -3532,24 +3571,24 @@
         <v>0</v>
       </c>
       <c r="P17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q17" t="s">
+        <v>18</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17" t="s">
         <v>19</v>
-      </c>
-      <c r="R17">
-        <v>0</v>
-      </c>
-      <c r="S17">
-        <v>0</v>
-      </c>
-      <c r="T17" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -3600,18 +3639,18 @@
         <v>0</v>
       </c>
       <c r="R18" t="s">
+        <v>18</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18" t="s">
         <v>19</v>
-      </c>
-      <c r="S18">
-        <v>0</v>
-      </c>
-      <c r="T18" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -3673,7 +3712,7 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20">
         <v>0</v>

</xml_diff>

<commit_message>
Update and refactor with TCA/IRC
</commit_message>
<xml_diff>
--- a/models/markov.xlsx
+++ b/models/markov.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\david\anus\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0051CCF-BD26-4130-BA49-6F9AA3AACB01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51426AC-A940-45A6-906A-1B805A6A2549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46680" yWindow="2790" windowWidth="19440" windowHeight="15600" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -167,45 +167,6 @@
     <t>p_survive</t>
   </si>
   <si>
-    <t>semestral_followup1_irc_no_hsil</t>
-  </si>
-  <si>
-    <t>semestral_followup2_irc_no_hsil</t>
-  </si>
-  <si>
-    <t>semestral_followup1_irc_hsil</t>
-  </si>
-  <si>
-    <t>semestral_followup2_irc_hsil</t>
-  </si>
-  <si>
-    <t>Semestral followup (1) (no HSIL, IRC treatment)</t>
-  </si>
-  <si>
-    <t>Semestral followup (2) (no HSIL, IRC treatment)</t>
-  </si>
-  <si>
-    <t>Semestral followup (1) (HSIL, IRC treatment)</t>
-  </si>
-  <si>
-    <t>Semestral followup (2) (HSIL, IRC treatment)</t>
-  </si>
-  <si>
-    <t>p_semestral_followup_irc___no_hsil</t>
-  </si>
-  <si>
-    <t>p_semestral_followup_irc___hsil</t>
-  </si>
-  <si>
-    <t>p_hsil___semestral_followup_no_hsil_irc</t>
-  </si>
-  <si>
-    <t>p_hsil_detected___semestral_followup_no_hsil_irc</t>
-  </si>
-  <si>
-    <t>p_hsil_detected___semestral_followup_hsil_irc</t>
-  </si>
-  <si>
     <t>p_cancer___undetected_hsil</t>
   </si>
   <si>
@@ -227,21 +188,6 @@
     <t>p_surgery_no_cancer___semestral_followup_hsil</t>
   </si>
   <si>
-    <t>p_surgery_no_cancer___semestral_followup_irc_no_hsil</t>
-  </si>
-  <si>
-    <t>p_surgery_no_cancer___semestral_followup_irc_hsil</t>
-  </si>
-  <si>
-    <t>p_cancer___semestral_followup_irc_hsil</t>
-  </si>
-  <si>
-    <t>u_hiv_p___irc</t>
-  </si>
-  <si>
-    <t>u_hsil___irc</t>
-  </si>
-  <si>
     <t>u_surgery_no_cancer</t>
   </si>
   <si>
@@ -267,9 +213,6 @@
   </si>
   <si>
     <t>p_hsil_regression___semestral_followup_hsil</t>
-  </si>
-  <si>
-    <t>p_hsil_regression___semestral_followup_hsil_irc</t>
   </si>
   <si>
     <r>
@@ -312,6 +255,63 @@
       </rPr>
       <t>(no HSIL)</t>
     </r>
+  </si>
+  <si>
+    <t>semestral_followup1_treatment_no_hsil</t>
+  </si>
+  <si>
+    <t>semestral_followup2_treatment_no_hsil</t>
+  </si>
+  <si>
+    <t>semestral_followup1_treatment_hsil</t>
+  </si>
+  <si>
+    <t>semestral_followup2_treatment_hsil</t>
+  </si>
+  <si>
+    <t>Semestral followup (1) (no HSIL, IRC/TCA/... treatment)</t>
+  </si>
+  <si>
+    <t>Semestral followup (2) (no HSIL, IRC/TCA/... treatment)</t>
+  </si>
+  <si>
+    <t>Semestral followup (1) (HSIL, IRC/TCA/... treatment)</t>
+  </si>
+  <si>
+    <t>Semestral followup (2) (HSIL, IRC/TCA/... treatment)</t>
+  </si>
+  <si>
+    <t>u_hiv_p___treatment</t>
+  </si>
+  <si>
+    <t>u_hsil___treatment</t>
+  </si>
+  <si>
+    <t>p_hsil___semestral_followup_no_hsil_treatment</t>
+  </si>
+  <si>
+    <t>p_hsil_regression___semestral_followup_hsil_treatment</t>
+  </si>
+  <si>
+    <t>p_hsil_detected___semestral_followup_no_hsil_treatment</t>
+  </si>
+  <si>
+    <t>p_hsil_detected___semestral_followup_hsil_treatment</t>
+  </si>
+  <si>
+    <t>p_surgery_no_cancer___semestral_followup_treatment_no_hsil</t>
+  </si>
+  <si>
+    <t>p_surgery_no_cancer___semestral_followup_treatment_hsil</t>
+  </si>
+  <si>
+    <t>p_cancer___semestral_followup_treatment_hsil</t>
+  </si>
+  <si>
+    <t>p_semestral_followup_treatment___no_hsil</t>
+  </si>
+  <si>
+    <t>p_semestral_followup_treatment___hsil</t>
   </si>
 </sst>
 </file>
@@ -388,9 +388,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -428,7 +428,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -534,7 +534,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -676,7 +676,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -687,7 +687,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A12" sqref="A12:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -717,7 +717,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -728,10 +728,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -742,10 +742,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -770,10 +770,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -784,10 +784,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -854,58 +854,58 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -938,16 +938,16 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -992,18 +992,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
     <col min="3" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
     <col min="6" max="7" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="18" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
     <col min="10" max="10" width="20.5703125" customWidth="1"/>
     <col min="11" max="11" width="20.85546875" customWidth="1"/>
     <col min="12" max="13" width="26.85546875" bestFit="1" customWidth="1"/>
@@ -1022,19 +1023,19 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="E1" t="s">
         <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="G1" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -1049,16 +1050,16 @@
         <v>29</v>
       </c>
       <c r="L1" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="M1" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="N1" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="O1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="P1" t="s">
         <v>6</v>
@@ -1067,7 +1068,7 @@
         <v>9</v>
       </c>
       <c r="R1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="S1" t="s">
         <v>12</v>
@@ -1086,12 +1087,12 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
@@ -1104,12 +1105,12 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
@@ -1149,22 +1150,22 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
@@ -1194,7 +1195,7 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
@@ -1224,14 +1225,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
@@ -1262,19 +1263,19 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="E1" t="s">
         <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="G1" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -1289,16 +1290,16 @@
         <v>29</v>
       </c>
       <c r="L1" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="M1" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="N1" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="O1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="P1" t="s">
         <v>6</v>
@@ -1307,7 +1308,7 @@
         <v>9</v>
       </c>
       <c r="R1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="S1" t="s">
         <v>12</v>
@@ -1351,7 +1352,7 @@
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -1369,7 +1370,7 @@
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="S2">
         <v>0</v>
@@ -1380,7 +1381,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1442,7 +1443,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1543,19 +1544,19 @@
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="Q5">
         <v>0</v>
       </c>
       <c r="R5" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="S5">
         <v>0</v>
@@ -1566,7 +1567,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1628,7 +1629,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1723,7 +1724,7 @@
         <v>0</v>
       </c>
       <c r="L8" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -1741,7 +1742,7 @@
         <v>0</v>
       </c>
       <c r="R8" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="S8">
         <v>0</v>
@@ -1785,7 +1786,7 @@
         <v>0</v>
       </c>
       <c r="L9" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -1803,7 +1804,7 @@
         <v>0</v>
       </c>
       <c r="R9" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="S9">
         <v>0</v>
@@ -1853,7 +1854,7 @@
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -1865,7 +1866,7 @@
         <v>0</v>
       </c>
       <c r="R10" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="S10">
         <v>0</v>
@@ -1915,7 +1916,7 @@
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -1927,7 +1928,7 @@
         <v>0</v>
       </c>
       <c r="R11" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="S11">
         <v>0</v>
@@ -1938,7 +1939,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1971,7 +1972,7 @@
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="M12" t="s">
         <v>18</v>
@@ -1989,7 +1990,7 @@
         <v>0</v>
       </c>
       <c r="R12" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="S12">
         <v>0</v>
@@ -2000,7 +2001,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
         <v>18</v>
@@ -2033,7 +2034,7 @@
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -2051,7 +2052,7 @@
         <v>0</v>
       </c>
       <c r="R13" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="S13">
         <v>0</v>
@@ -2062,7 +2063,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -2101,19 +2102,19 @@
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="O14" t="s">
         <v>18</v>
       </c>
       <c r="P14" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="Q14">
         <v>0</v>
       </c>
       <c r="R14" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="S14">
         <v>0</v>
@@ -2124,7 +2125,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -2163,19 +2164,19 @@
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="Q15">
         <v>0</v>
       </c>
       <c r="R15" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="S15">
         <v>0</v>
@@ -2310,7 +2311,7 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -2508,27 +2509,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0EB2218-1218-4D74-BE4B-A50C70982977}">
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E3" sqref="E3"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="30.28515625" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" customWidth="1"/>
-    <col min="6" max="7" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="37.140625" customWidth="1"/>
-    <col min="17" max="18" width="16.42578125" customWidth="1"/>
-    <col min="19" max="19" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="38" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="41" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="19.5703125" customWidth="1"/>
     <col min="22" max="22" width="22" customWidth="1"/>
     <col min="23" max="23" width="14.5703125" customWidth="1"/>
@@ -2540,19 +2541,19 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="E1" t="s">
         <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="G1" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
@@ -2567,16 +2568,16 @@
         <v>29</v>
       </c>
       <c r="L1" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="M1" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="N1" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="O1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="P1" t="s">
         <v>6</v>
@@ -2585,7 +2586,7 @@
         <v>9</v>
       </c>
       <c r="R1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="S1" t="s">
         <v>12</v>
@@ -2658,7 +2659,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2720,7 +2721,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -2785,7 +2786,7 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -2844,10 +2845,10 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -2906,10 +2907,10 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -3113,7 +3114,7 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -3178,7 +3179,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -3216,7 +3217,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -3255,7 +3256,7 @@
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="O12">
         <v>0</v>
@@ -3278,7 +3279,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -3320,7 +3321,7 @@
         <v>0</v>
       </c>
       <c r="O13" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="P13">
         <v>0</v>
@@ -3340,7 +3341,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -3373,7 +3374,7 @@
         <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -3402,7 +3403,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -3438,7 +3439,7 @@
         <v>0</v>
       </c>
       <c r="M15" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="N15">
         <v>0</v>
@@ -3588,7 +3589,7 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B18">
         <v>0</v>

</xml_diff>

<commit_message>
Add changes to model and model calibration
</commit_message>
<xml_diff>
--- a/models/markov.xlsx
+++ b/models/markov.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\david\anus\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51426AC-A940-45A6-906A-1B805A6A2549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572F2593-3EF1-4C4F-8C9B-C691FDC75307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="84">
   <si>
     <t>name</t>
   </si>
@@ -312,6 +312,18 @@
   </si>
   <si>
     <t>p_semestral_followup_treatment___hsil</t>
+  </si>
+  <si>
+    <t>cancer_delayed</t>
+  </si>
+  <si>
+    <t>Anal cancer (delayed diagnosis)</t>
+  </si>
+  <si>
+    <t>u_cancer_delayed</t>
+  </si>
+  <si>
+    <t>p_death_cancer_delayed</t>
   </si>
 </sst>
 </file>
@@ -684,21 +696,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:A15"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="33.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.54296875" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -712,7 +724,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -726,7 +738,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -740,7 +752,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -754,7 +766,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -768,7 +780,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -782,7 +794,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -796,7 +808,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -810,7 +822,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -824,7 +836,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -838,7 +850,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -852,7 +864,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>61</v>
       </c>
@@ -866,7 +878,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -880,7 +892,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -894,7 +906,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -908,7 +920,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -922,59 +934,73 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>9</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>10</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>43</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>44</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>12</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>13</v>
       </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>14</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>15</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
         <v>0</v>
       </c>
     </row>
@@ -990,35 +1016,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="7" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="3" max="4" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" customWidth="1"/>
+    <col min="6" max="7" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.81640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" customWidth="1"/>
-    <col min="11" max="11" width="20.85546875" customWidth="1"/>
-    <col min="12" max="13" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" customWidth="1"/>
-    <col min="17" max="18" width="19.5703125" customWidth="1"/>
-    <col min="19" max="19" width="14.85546875" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" customWidth="1"/>
-    <col min="21" max="21" width="19.5703125" customWidth="1"/>
-    <col min="22" max="22" width="12.7109375" customWidth="1"/>
-    <col min="23" max="23" width="11.28515625" customWidth="1"/>
+    <col min="10" max="10" width="20.54296875" customWidth="1"/>
+    <col min="11" max="11" width="20.81640625" customWidth="1"/>
+    <col min="12" max="13" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7265625" customWidth="1"/>
+    <col min="17" max="17" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="19.54296875" customWidth="1"/>
+    <col min="20" max="20" width="14.81640625" customWidth="1"/>
+    <col min="21" max="21" width="13.7265625" customWidth="1"/>
+    <col min="22" max="22" width="19.54296875" customWidth="1"/>
+    <col min="23" max="23" width="12.7265625" customWidth="1"/>
+    <col min="24" max="24" width="11.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -1065,149 +1092,157 @@
         <v>6</v>
       </c>
       <c r="Q1" t="s">
+        <v>80</v>
+      </c>
+      <c r="R1" t="s">
         <v>9</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>43</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>12</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
-      <c r="T11" t="s">
+      <c r="U11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="R16" t="s">
         <v>9</v>
       </c>
-      <c r="S16" t="s">
+      <c r="T16" t="s">
         <v>17</v>
       </c>
-      <c r="T16" t="s">
+      <c r="U16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>9</v>
       </c>
-      <c r="P17" t="s">
+      <c r="P18" t="s">
         <v>36</v>
       </c>
-      <c r="T17" t="s">
+      <c r="U18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>12</v>
       </c>
-      <c r="T19" t="s">
+      <c r="U20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1223,42 +1258,43 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M13" sqref="M13"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" customWidth="1"/>
-    <col min="8" max="8" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.42578125" customWidth="1"/>
-    <col min="14" max="14" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.42578125" customWidth="1"/>
-    <col min="16" max="16" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.42578125" customWidth="1"/>
-    <col min="18" max="18" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.42578125" customWidth="1"/>
-    <col min="20" max="20" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.5703125" customWidth="1"/>
-    <col min="22" max="22" width="22" customWidth="1"/>
-    <col min="23" max="23" width="14.5703125" customWidth="1"/>
-    <col min="1033" max="1036" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.1796875" customWidth="1"/>
+    <col min="8" max="8" width="39.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="41.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.453125" customWidth="1"/>
+    <col min="14" max="14" width="38.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.453125" customWidth="1"/>
+    <col min="16" max="16" width="33.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.26953125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.453125" customWidth="1"/>
+    <col min="19" max="19" width="46.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.453125" customWidth="1"/>
+    <col min="21" max="21" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.54296875" customWidth="1"/>
+    <col min="23" max="23" width="22" customWidth="1"/>
+    <col min="24" max="24" width="14.54296875" customWidth="1"/>
+    <col min="1034" max="1037" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -1305,19 +1341,22 @@
         <v>6</v>
       </c>
       <c r="Q1" t="s">
+        <v>80</v>
+      </c>
+      <c r="R1" t="s">
         <v>9</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>43</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>12</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1369,17 +1408,20 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2" t="s">
         <v>45</v>
       </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
       <c r="T2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -1440,8 +1482,11 @@
       <c r="T3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -1502,8 +1547,11 @@
       <c r="T4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1549,23 +1597,26 @@
       <c r="O5">
         <v>0</v>
       </c>
-      <c r="P5" t="s">
-        <v>42</v>
+      <c r="P5">
+        <v>0</v>
       </c>
       <c r="Q5">
         <v>0</v>
       </c>
-      <c r="R5" t="s">
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5" t="s">
         <v>46</v>
       </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
       <c r="T5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -1626,8 +1677,11 @@
       <c r="T6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -1688,8 +1742,11 @@
       <c r="T7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1741,17 +1798,20 @@
       <c r="Q8">
         <v>0</v>
       </c>
-      <c r="R8" t="s">
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8" t="s">
         <v>47</v>
       </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
       <c r="T8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1803,17 +1863,20 @@
       <c r="Q9">
         <v>0</v>
       </c>
-      <c r="R9" t="s">
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9" t="s">
         <v>47</v>
       </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
       <c r="T9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1865,17 +1928,20 @@
       <c r="Q10">
         <v>0</v>
       </c>
-      <c r="R10" t="s">
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10" t="s">
         <v>48</v>
       </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
       <c r="T10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1927,17 +1993,20 @@
       <c r="Q11">
         <v>0</v>
       </c>
-      <c r="R11" t="s">
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11" t="s">
         <v>48</v>
       </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
       <c r="T11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>61</v>
       </c>
@@ -1989,17 +2058,20 @@
       <c r="Q12">
         <v>0</v>
       </c>
-      <c r="R12" t="s">
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12" t="s">
         <v>75</v>
       </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
       <c r="T12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -2051,17 +2123,20 @@
       <c r="Q13">
         <v>0</v>
       </c>
-      <c r="R13" t="s">
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13" t="s">
         <v>75</v>
       </c>
-      <c r="S13">
-        <v>0</v>
-      </c>
       <c r="T13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -2113,17 +2188,20 @@
       <c r="Q14">
         <v>0</v>
       </c>
-      <c r="R14" t="s">
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14" t="s">
         <v>76</v>
       </c>
-      <c r="S14">
-        <v>0</v>
-      </c>
       <c r="T14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -2175,17 +2253,20 @@
       <c r="Q15">
         <v>0</v>
       </c>
-      <c r="R15" t="s">
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15" t="s">
         <v>76</v>
       </c>
-      <c r="S15">
-        <v>0</v>
-      </c>
       <c r="T15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -2246,10 +2327,13 @@
       <c r="T16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -2308,10 +2392,13 @@
       <c r="T17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -2370,10 +2457,13 @@
       <c r="T18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -2432,66 +2522,137 @@
       <c r="T19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>1</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>14</v>
       </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
-      <c r="R20">
-        <v>0</v>
-      </c>
-      <c r="S20">
-        <v>0</v>
-      </c>
-      <c r="T20">
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
         <v>1</v>
       </c>
     </row>
@@ -2507,36 +2668,37 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0EB2218-1218-4D74-BE4B-A50C70982977}">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M7" sqref="M7"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="28.81640625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="38" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="31.453125" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="41" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.5703125" customWidth="1"/>
-    <col min="22" max="22" width="22" customWidth="1"/>
-    <col min="23" max="23" width="14.5703125" customWidth="1"/>
-    <col min="1033" max="1036" width="11.5703125" customWidth="1"/>
+    <col min="14" max="15" width="34.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.453125" customWidth="1"/>
+    <col min="18" max="18" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.54296875" customWidth="1"/>
+    <col min="23" max="23" width="22" customWidth="1"/>
+    <col min="24" max="24" width="14.54296875" customWidth="1"/>
+    <col min="1034" max="1037" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -2583,19 +2745,22 @@
         <v>6</v>
       </c>
       <c r="Q1" t="s">
+        <v>80</v>
+      </c>
+      <c r="R1" t="s">
         <v>9</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>43</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>12</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2653,11 +2818,14 @@
       <c r="S2">
         <v>0</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -2715,11 +2883,14 @@
       <c r="S3">
         <v>0</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -2777,11 +2948,14 @@
       <c r="S4">
         <v>0</v>
       </c>
-      <c r="T4" t="s">
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -2830,8 +3004,8 @@
       <c r="P5">
         <v>0</v>
       </c>
-      <c r="Q5">
-        <v>0</v>
+      <c r="Q5" t="s">
+        <v>42</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -2839,11 +3013,14 @@
       <c r="S5">
         <v>0</v>
       </c>
-      <c r="T5" t="s">
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -2892,8 +3069,8 @@
       <c r="P6">
         <v>0</v>
       </c>
-      <c r="Q6">
-        <v>0</v>
+      <c r="Q6" t="s">
+        <v>42</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -2901,11 +3078,14 @@
       <c r="S6">
         <v>0</v>
       </c>
-      <c r="T6" t="s">
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -2954,8 +3134,8 @@
       <c r="P7">
         <v>0</v>
       </c>
-      <c r="Q7">
-        <v>0</v>
+      <c r="Q7" t="s">
+        <v>42</v>
       </c>
       <c r="R7">
         <v>0</v>
@@ -2963,11 +3143,14 @@
       <c r="S7">
         <v>0</v>
       </c>
-      <c r="T7" t="s">
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -3025,11 +3208,14 @@
       <c r="S8">
         <v>0</v>
       </c>
-      <c r="T8" t="s">
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -3087,11 +3273,14 @@
       <c r="S9">
         <v>0</v>
       </c>
-      <c r="T9" t="s">
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -3149,11 +3338,14 @@
       <c r="S10">
         <v>0</v>
       </c>
-      <c r="T10" t="s">
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -3211,11 +3403,14 @@
       <c r="S11">
         <v>0</v>
       </c>
-      <c r="T11" t="s">
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>61</v>
       </c>
@@ -3273,11 +3468,14 @@
       <c r="S12">
         <v>0</v>
       </c>
-      <c r="T12" t="s">
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -3335,11 +3533,14 @@
       <c r="S13">
         <v>0</v>
       </c>
-      <c r="T13" t="s">
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -3397,11 +3598,14 @@
       <c r="S14">
         <v>0</v>
       </c>
-      <c r="T14" t="s">
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -3459,11 +3663,14 @@
       <c r="S15">
         <v>0</v>
       </c>
-      <c r="T15" t="s">
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -3512,22 +3719,25 @@
       <c r="P16" t="s">
         <v>18</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16" t="s">
         <v>41</v>
       </c>
-      <c r="R16">
-        <v>0</v>
-      </c>
-      <c r="S16" t="s">
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16" t="s">
         <v>20</v>
       </c>
-      <c r="T16" t="s">
+      <c r="U16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -3571,8 +3781,8 @@
       <c r="O17">
         <v>0</v>
       </c>
-      <c r="P17" t="s">
-        <v>21</v>
+      <c r="P17">
+        <v>0</v>
       </c>
       <c r="Q17" t="s">
         <v>18</v>
@@ -3584,12 +3794,15 @@
         <v>0</v>
       </c>
       <c r="T17" t="s">
+        <v>83</v>
+      </c>
+      <c r="U17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -3633,8 +3846,8 @@
       <c r="O18">
         <v>0</v>
       </c>
-      <c r="P18">
-        <v>0</v>
+      <c r="P18" t="s">
+        <v>21</v>
       </c>
       <c r="Q18">
         <v>0</v>
@@ -3645,131 +3858,205 @@
       <c r="S18">
         <v>0</v>
       </c>
-      <c r="T18" t="s">
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19" t="s">
+        <v>18</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>12</v>
       </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
-      <c r="Q19">
-        <v>0</v>
-      </c>
-      <c r="R19">
-        <v>0</v>
-      </c>
-      <c r="S19">
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
         <v>1</v>
       </c>
-      <c r="T19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="U20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>14</v>
       </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
-      <c r="R20">
-        <v>0</v>
-      </c>
-      <c r="S20">
-        <v>0</v>
-      </c>
-      <c r="T20">
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
         <v>1</v>
       </c>
     </row>

</xml_diff>